<commit_message>
Update and add text classification
</commit_message>
<xml_diff>
--- a/models_performance.xlsx
+++ b/models_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\Facultate_anul_4\Licenta\ml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9163FE-0D3C-4071-93A6-BAF0C8BEBB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25565182-CE8E-496A-9DD0-1BB88A893A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="28">
   <si>
     <t>L</t>
   </si>
@@ -82,6 +82,33 @@
   </si>
   <si>
     <t>RONEC</t>
+  </si>
+  <si>
+    <t>NER</t>
+  </si>
+  <si>
+    <t>Adam(lr=1e-4)</t>
+  </si>
+  <si>
+    <t>Text classification</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>en_text_classification + en_personas</t>
+  </si>
+  <si>
+    <t>Embedding_output_dim</t>
+  </si>
+  <si>
+    <t>rnn_bidirectional_en</t>
+  </si>
+  <si>
+    <t>Adam(lr=1e-5)</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
 </sst>
 </file>
@@ -417,24 +444,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" customWidth="1"/>
     <col min="11" max="11" width="49.44140625" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="33.33203125" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -477,8 +508,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="16.2" customHeight="1">
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16.2" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -522,7 +556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -566,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -610,7 +644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -654,7 +688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -698,7 +732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -742,7 +776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -766,6 +800,308 @@
       </c>
       <c r="N8" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>256</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.88339999999999996</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.68779999999999997</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.63490000000000002</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.4577</v>
+      </c>
+      <c r="J9" s="2">
+        <v>11178785</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="3">
+        <v>32</v>
+      </c>
+      <c r="M9" s="3">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" t="s">
+        <v>16</v>
+      </c>
+      <c r="N19" t="s">
+        <v>13</v>
+      </c>
+      <c r="P19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <v>64</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.92049999999999998</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.90010000000000001</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1.5924</v>
+      </c>
+      <c r="J20" s="2">
+        <v>34254</v>
+      </c>
+      <c r="K20" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20">
+        <v>12</v>
+      </c>
+      <c r="N20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>64</v>
+      </c>
+      <c r="D21">
+        <v>64</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.93149999999999999</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.92020000000000002</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.92020000000000002</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.91259999999999997</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1.2462</v>
+      </c>
+      <c r="J21" s="2">
+        <v>76366</v>
+      </c>
+      <c r="K21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21">
+        <v>12</v>
+      </c>
+      <c r="N21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>64</v>
+      </c>
+      <c r="D22">
+        <v>64</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.64380000000000004</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.72060000000000002</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.72060000000000002</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.74050000000000005</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.99909999999999999</v>
+      </c>
+      <c r="J22" s="2">
+        <v>175182</v>
+      </c>
+      <c r="K22" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22">
+        <v>12</v>
+      </c>
+      <c r="N22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" t="s">
+        <v>13</v>
+      </c>
+      <c r="P28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>256</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.97170000000000001</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.97409999999999997</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.97409999999999997</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.23710000000000001</v>
+      </c>
+      <c r="J29" s="2">
+        <v>11174159</v>
+      </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" s="3">
+        <v>12</v>
+      </c>
+      <c r="M29" s="3">
+        <v>128</v>
+      </c>
+      <c r="N29" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>